<commit_message>
fix ch 1 files
</commit_message>
<xml_diff>
--- a/ch_01/ch_01_solutions.xlsx
+++ b/ch_01/ch_01_solutions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\GitHub\modern-analytics-excel-book\ch_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMount\Documents\GitHub\modern-analytics-excel-book\ch_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9EFD1C-9371-4894-BD2E-F1A20E2C08D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036602C6-43CF-4F43-9BA2-AD3E10F823F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="12676" xr2:uid="{27C0F9AC-F68D-4387-AFAA-DF2C8506B82D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{27C0F9AC-F68D-4387-AFAA-DF2C8506B82D}"/>
   </bookViews>
   <sheets>
     <sheet name="start" sheetId="3" r:id="rId1"/>
@@ -22,8 +22,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -13112,7 +13112,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{93F498C0-6251-4965-8460-389D7C36BCD6}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{93F498C0-6251-4965-8460-389D7C36BCD6}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H1:J18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -13135,7 +13135,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C45A1B19-F0B2-4A5B-A2D0-9F6384A092AA}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C45A1B19-F0B2-4A5B-A2D0-9F6384A092AA}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G1:I18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>

</xml_diff>